<commit_message>
corrige tablas sección 03
</commit_message>
<xml_diff>
--- a/data/tabla 03-10.xlsx
+++ b/data/tabla 03-10.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>2010</t>
   </si>
@@ -73,10 +73,894 @@
   <numFmts count="1">
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="443">
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
+  <fonts count="664">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1847,7 +2731,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="96">
+  <fills count="143">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2324,8 +3208,243 @@
         <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="353">
+  <borders count="529">
     <border>
       <left/>
       <right/>
@@ -5017,11 +6136,1353 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="353">
+  <cellXfs count="529">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -6428,6 +8889,710 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="442" fillId="95" borderId="352" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="443" fillId="0" borderId="353" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="444" fillId="0" borderId="354" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="445" fillId="0" borderId="355" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="446" fillId="0" borderId="356" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="447" fillId="0" borderId="357" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="448" fillId="0" borderId="358" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="449" fillId="0" borderId="359" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="450" fillId="0" borderId="360" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="451" fillId="0" borderId="361" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="452" fillId="0" borderId="362" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="453" fillId="0" borderId="363" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="454" fillId="0" borderId="364" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="455" fillId="0" borderId="365" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="456" fillId="0" borderId="366" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="457" fillId="0" borderId="367" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="458" fillId="0" borderId="368" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="459" fillId="0" borderId="369" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="460" fillId="0" borderId="370" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="461" fillId="0" borderId="371" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="462" fillId="0" borderId="372" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="463" fillId="0" borderId="373" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="464" fillId="0" borderId="374" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="465" fillId="0" borderId="375" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="466" fillId="0" borderId="376" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="467" fillId="0" borderId="377" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="468" fillId="0" borderId="378" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="469" fillId="0" borderId="379" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="470" fillId="0" borderId="380" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="471" fillId="0" borderId="381" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="472" fillId="0" borderId="382" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="473" fillId="0" borderId="383" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="474" fillId="0" borderId="384" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="475" fillId="0" borderId="385" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="476" fillId="0" borderId="386" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="477" fillId="0" borderId="387" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="478" fillId="0" borderId="388" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="479" fillId="0" borderId="389" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="480" fillId="0" borderId="390" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="481" fillId="0" borderId="391" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="482" fillId="0" borderId="392" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="483" fillId="0" borderId="393" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="484" fillId="0" borderId="394" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="485" fillId="0" borderId="395" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="486" fillId="0" borderId="396" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="487" fillId="0" borderId="397" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="488" fillId="0" borderId="398" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="489" fillId="0" borderId="399" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="490" fillId="0" borderId="400" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="491" fillId="0" borderId="401" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="492" fillId="0" borderId="402" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="493" fillId="0" borderId="403" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="494" fillId="0" borderId="404" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="495" fillId="0" borderId="405" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="496" fillId="0" borderId="406" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="497" fillId="0" borderId="407" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="498" fillId="0" borderId="408" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="499" fillId="0" borderId="409" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="500" fillId="0" borderId="410" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="501" fillId="0" borderId="411" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="502" fillId="0" borderId="412" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="503" fillId="0" borderId="413" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="504" fillId="0" borderId="414" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="505" fillId="0" borderId="415" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="506" fillId="0" borderId="416" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="507" fillId="0" borderId="417" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="508" fillId="0" borderId="418" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="509" fillId="0" borderId="419" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="510" fillId="0" borderId="420" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="511" fillId="0" borderId="421" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="512" fillId="0" borderId="422" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="513" fillId="0" borderId="423" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="514" fillId="0" borderId="424" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="515" fillId="0" borderId="425" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="516" fillId="0" borderId="426" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="517" fillId="0" borderId="427" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="518" fillId="0" borderId="428" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="519" fillId="0" borderId="429" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="520" fillId="0" borderId="430" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="521" fillId="0" borderId="431" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="522" fillId="0" borderId="432" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="523" fillId="0" borderId="433" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="524" fillId="0" borderId="434" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="525" fillId="0" borderId="435" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="526" fillId="0" borderId="436" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="528" fillId="0" borderId="437" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="530" fillId="0" borderId="438" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="532" fillId="0" borderId="439" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="534" fillId="0" borderId="440" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="536" fillId="0" borderId="441" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="538" fillId="0" borderId="442" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="540" fillId="0" borderId="443" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="542" fillId="0" borderId="444" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="544" fillId="0" borderId="445" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="546" fillId="0" borderId="446" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="548" fillId="0" borderId="447" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="550" fillId="0" borderId="448" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="552" fillId="0" borderId="449" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="554" fillId="0" borderId="450" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="556" fillId="0" borderId="451" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="558" fillId="0" borderId="452" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="560" fillId="0" borderId="453" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="562" fillId="0" borderId="454" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="564" fillId="0" borderId="455" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="566" fillId="0" borderId="456" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="568" fillId="0" borderId="457" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="570" fillId="0" borderId="458" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="572" fillId="0" borderId="459" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="574" fillId="0" borderId="460" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="576" fillId="0" borderId="461" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="578" fillId="0" borderId="462" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="580" fillId="0" borderId="463" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="582" fillId="0" borderId="464" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="584" fillId="0" borderId="465" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="586" fillId="0" borderId="466" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="588" fillId="0" borderId="467" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="590" fillId="0" borderId="468" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="592" fillId="0" borderId="469" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="594" fillId="0" borderId="470" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="596" fillId="0" borderId="471" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="598" fillId="0" borderId="472" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="600" fillId="0" borderId="473" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="602" fillId="0" borderId="474" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="604" fillId="0" borderId="475" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="606" fillId="0" borderId="476" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="608" fillId="0" borderId="477" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="610" fillId="0" borderId="478" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="612" fillId="0" borderId="479" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="614" fillId="0" borderId="480" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="616" fillId="0" borderId="481" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="617" fillId="96" borderId="482" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="618" fillId="97" borderId="483" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="619" fillId="98" borderId="484" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="620" fillId="99" borderId="485" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="621" fillId="100" borderId="486" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="622" fillId="101" borderId="487" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="623" fillId="102" borderId="488" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="624" fillId="103" borderId="489" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="625" fillId="104" borderId="490" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="626" fillId="105" borderId="491" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="627" fillId="106" borderId="492" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="628" fillId="107" borderId="493" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="629" fillId="108" borderId="494" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="630" fillId="109" borderId="495" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="631" fillId="110" borderId="496" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="632" fillId="111" borderId="497" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="633" fillId="112" borderId="498" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="634" fillId="113" borderId="499" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="635" fillId="114" borderId="500" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="636" fillId="115" borderId="501" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="637" fillId="116" borderId="502" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="638" fillId="117" borderId="503" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="639" fillId="118" borderId="504" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="640" fillId="119" borderId="505" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="641" fillId="120" borderId="506" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="642" fillId="121" borderId="507" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="643" fillId="122" borderId="508" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="644" fillId="123" borderId="509" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="645" fillId="124" borderId="510" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="646" fillId="125" borderId="511" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="647" fillId="126" borderId="512" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="648" fillId="127" borderId="513" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="649" fillId="128" borderId="514" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="650" fillId="129" borderId="515" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="651" fillId="130" borderId="516" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="652" fillId="131" borderId="517" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="653" fillId="132" borderId="518" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="654" fillId="133" borderId="519" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="655" fillId="134" borderId="520" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="656" fillId="135" borderId="521" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="657" fillId="136" borderId="522" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="658" fillId="137" borderId="523" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="49" fontId="659" fillId="138" borderId="524" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="660" fillId="139" borderId="525" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="661" fillId="140" borderId="526" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="662" fillId="141" borderId="527" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="663" fillId="142" borderId="528" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6444,167 +9609,167 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
-      <c r="A2" s="306" t="s">
+      <c r="A2" s="482" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="351" t="s">
+      <c r="B2" s="527" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="352" t="s">
+      <c r="C2" s="528" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="309" t="s">
+      <c r="A3" s="485" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="310">
+      <c r="B3" s="486">
         <v>44.442291259765625</v>
       </c>
-      <c r="C3" s="311">
+      <c r="C3" s="487">
         <v>47.719284057617188</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="312" t="s">
+      <c r="A4" s="488" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="313">
+      <c r="B4" s="489">
         <v>40.811019897460937</v>
       </c>
-      <c r="C4" s="314">
+      <c r="C4" s="490">
         <v>42.067115783691406</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="315" t="s">
+      <c r="A5" s="491" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="316">
+      <c r="B5" s="492">
         <v>39.693977355957031</v>
       </c>
-      <c r="C5" s="317">
+      <c r="C5" s="493">
         <v>40.825035095214844</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="318" t="s">
+      <c r="A6" s="494" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="319">
+      <c r="B6" s="495">
         <v>41.296875</v>
       </c>
-      <c r="C6" s="320">
+      <c r="C6" s="496">
         <v>43.102630615234375</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="321" t="s">
+      <c r="A7" s="497" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="322">
+      <c r="B7" s="498">
         <v>39.431659698486328</v>
       </c>
-      <c r="C7" s="323">
+      <c r="C7" s="499">
         <v>41.326839447021484</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="324" t="s">
+      <c r="A8" s="500" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="325">
+      <c r="B8" s="501">
         <v>41.958854675292969</v>
       </c>
-      <c r="C8" s="326">
+      <c r="C8" s="502">
         <v>43.162033081054687</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="327" t="s">
+      <c r="A9" s="503" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="328">
+      <c r="B9" s="504">
         <v>40.746719360351563</v>
       </c>
-      <c r="C9" s="329">
+      <c r="C9" s="505">
         <v>42.076927185058594</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="330" t="s">
+      <c r="A10" s="506" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="331">
+      <c r="B10" s="507">
         <v>37.807415008544922</v>
       </c>
-      <c r="C10" s="332">
+      <c r="C10" s="508">
         <v>38.648078918457031</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="333" t="s">
+      <c r="A11" s="509" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="334">
+      <c r="B11" s="510">
         <v>41.932701110839844</v>
       </c>
-      <c r="C11" s="335">
+      <c r="C11" s="511">
         <v>44.16339111328125</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="336" t="s">
+      <c r="A12" s="512" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="337">
+      <c r="B12" s="513">
         <v>40.014469146728516</v>
       </c>
-      <c r="C12" s="338">
+      <c r="C12" s="514">
         <v>42.100532531738281</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="339" t="s">
+      <c r="A13" s="515" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="340">
+      <c r="B13" s="516">
         <v>39.424163818359375</v>
       </c>
-      <c r="C13" s="341">
+      <c r="C13" s="517">
         <v>41.701690673828125</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="342" t="s">
+      <c r="A14" s="518" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="343">
+      <c r="B14" s="519">
         <v>42.797233581542969</v>
       </c>
-      <c r="C14" s="344">
+      <c r="C14" s="520">
         <v>44.011848449707031</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="345" t="s">
+      <c r="A15" s="521" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="346">
+      <c r="B15" s="522">
         <v>41.78717041015625</v>
       </c>
-      <c r="C15" s="347">
+      <c r="C15" s="523">
         <v>43.143714904785156</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="348" t="s">
+      <c r="A16" s="524" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="349">
+      <c r="B16" s="525">
         <v>41.605014801025391</v>
       </c>
-      <c r="C16" s="350">
+      <c r="C16" s="526">
         <v>43.212192535400391</v>
       </c>
     </row>

</xml_diff>